<commit_message>
feat(analysis/): results presented on 9 Feb
</commit_message>
<xml_diff>
--- a/analysis/2026/summary_CoT.xlsx
+++ b/analysis/2026/summary_CoT.xlsx
@@ -66,13 +66,13 @@
     <t>gemini-2.5-flash</t>
   </si>
   <si>
-    <t>cascade_Qwen-7B-Chat</t>
+    <t>cascade_qwen-7b-chat</t>
   </si>
   <si>
-    <t>cascade_Llama-3_1-8B-Instruct</t>
+    <t>cascade_llama-3_1-8b-instruct</t>
   </si>
   <si>
-    <t>cascade_Qwen25-7B-Instruct</t>
+    <t>cascade_qwen25-7b-instruct</t>
   </si>
   <si>
     <t>New Task Acc</t>

</xml_diff>